<commit_message>
added new stocks, fixed tc model
</commit_message>
<xml_diff>
--- a/etfs/ETF_Metrics_FullList.xlsx
+++ b/etfs/ETF_Metrics_FullList.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>Holdings Count</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -492,13 +497,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>79.55</v>
+        <v>88.02</v>
       </c>
       <c r="C2" t="n">
-        <v>17.04</v>
+        <v>17.58</v>
       </c>
       <c r="D2" t="n">
-        <v>45.4</v>
+        <v>45.59</v>
       </c>
       <c r="E2" t="n">
         <v>38.569</v>
@@ -512,6 +517,7 @@
         <v>8274846208</v>
       </c>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -520,10 +526,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23.16</v>
+        <v>25.09</v>
       </c>
       <c r="C3" t="n">
-        <v>17.94</v>
+        <v>18.33</v>
       </c>
       <c r="D3" t="n">
         <v>21.36</v>
@@ -540,6 +546,7 @@
         <v>3888684288</v>
       </c>
       <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -548,10 +555,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.76</v>
+        <v>17.71</v>
       </c>
       <c r="C4" t="n">
-        <v>8.58</v>
+        <v>8.32</v>
       </c>
       <c r="D4" t="n">
         <v>21.28</v>
@@ -568,6 +575,7 @@
         <v>182574192</v>
       </c>
       <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,13 +584,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.68</v>
+        <v>16.09</v>
       </c>
       <c r="C5" t="n">
-        <v>12.92</v>
+        <v>13.16</v>
       </c>
       <c r="D5" t="n">
-        <v>23.33</v>
+        <v>23.35</v>
       </c>
       <c r="E5" t="n">
         <v>32.65</v>
@@ -596,6 +604,7 @@
         <v>9603175424</v>
       </c>
       <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -604,10 +613,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25.31</v>
+        <v>26.18</v>
       </c>
       <c r="C6" t="n">
-        <v>4.98</v>
+        <v>5.3</v>
       </c>
       <c r="D6" t="n">
         <v>39.85</v>
@@ -624,6 +633,7 @@
         <v>785164864</v>
       </c>
       <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -631,27 +641,20 @@
           <t>PHO</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="C7" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>18.43</v>
-      </c>
-      <c r="E7" t="n">
-        <v>57.11</v>
-      </c>
-      <c r="F7" t="n">
-        <v>74.33</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>2243255808</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Failed to perform, curl: (23) Failure writing output to destination, passed 13 returned 0. See https://curl.se/libcurl/c/libcurl-errors.html first for more details.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -660,13 +663,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63.74</v>
+        <v>63.79</v>
       </c>
       <c r="C8" t="n">
-        <v>5.82</v>
+        <v>6.1</v>
       </c>
       <c r="D8" t="n">
-        <v>40.85</v>
+        <v>41.11</v>
       </c>
       <c r="E8" t="n">
         <v>13.19</v>
@@ -680,6 +683,7 @@
         <v>476309024</v>
       </c>
       <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -688,19 +692,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.88</v>
+        <v>8.56</v>
       </c>
       <c r="C9" t="n">
-        <v>4.15</v>
+        <v>4.6</v>
       </c>
       <c r="D9" t="n">
-        <v>23.47</v>
+        <v>23.48</v>
       </c>
       <c r="E9" t="n">
         <v>107.43</v>
       </c>
       <c r="F9" t="n">
-        <v>156.36</v>
+        <v>157.1893</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -708,6 +712,7 @@
         <v>5940781568</v>
       </c>
       <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -716,10 +721,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8.57</v>
+        <v>10.63</v>
       </c>
       <c r="C10" t="n">
-        <v>12.78</v>
+        <v>12.72</v>
       </c>
       <c r="D10" t="n">
         <v>15.02</v>
@@ -736,6 +741,7 @@
         <v>34413137920</v>
       </c>
       <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -744,13 +750,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14.41</v>
+        <v>16.17</v>
       </c>
       <c r="C11" t="n">
-        <v>13.1</v>
+        <v>13.23</v>
       </c>
       <c r="D11" t="n">
-        <v>19.35</v>
+        <v>19.37</v>
       </c>
       <c r="E11" t="n">
         <v>105.18</v>
@@ -764,6 +770,7 @@
         <v>14951828480</v>
       </c>
       <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -772,13 +779,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25.51</v>
+        <v>25.19</v>
       </c>
       <c r="C12" t="n">
-        <v>7.04</v>
+        <v>6.82</v>
       </c>
       <c r="D12" t="n">
-        <v>22.87</v>
+        <v>22.92</v>
       </c>
       <c r="E12" t="n">
         <v>10.46</v>
@@ -792,6 +799,7 @@
         <v>1679520128</v>
       </c>
       <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -800,19 +808,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-3.03</v>
+        <v>-1.29</v>
       </c>
       <c r="C13" t="n">
-        <v>7.63</v>
+        <v>7.51</v>
       </c>
       <c r="D13" t="n">
-        <v>14.39</v>
+        <v>14.35</v>
       </c>
       <c r="E13" t="n">
         <v>47.6</v>
       </c>
       <c r="F13" t="n">
-        <v>56.29</v>
+        <v>56.01</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -820,6 +828,7 @@
         <v>9142732800</v>
       </c>
       <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -828,13 +837,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>28.63</v>
+        <v>28.4</v>
       </c>
       <c r="C14" t="n">
-        <v>4.51</v>
+        <v>4.29</v>
       </c>
       <c r="D14" t="n">
-        <v>23.07</v>
+        <v>23.09</v>
       </c>
       <c r="E14" t="n">
         <v>46.41</v>
@@ -848,6 +857,7 @@
         <v>2198633216</v>
       </c>
       <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -856,19 +866,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>18.62</v>
+        <v>20.26</v>
       </c>
       <c r="C15" t="n">
-        <v>14.17</v>
+        <v>14.25</v>
       </c>
       <c r="D15" t="n">
-        <v>25.85</v>
+        <v>25.89</v>
       </c>
       <c r="E15" t="n">
         <v>39.44</v>
       </c>
       <c r="F15" t="n">
-        <v>65.78</v>
+        <v>66.44</v>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -876,6 +886,7 @@
         <v>6578223616</v>
       </c>
       <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -884,13 +895,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>34.21</v>
+        <v>43.07</v>
       </c>
       <c r="C16" t="n">
-        <v>15.05</v>
+        <v>15.11</v>
       </c>
       <c r="D16" t="n">
-        <v>22.15</v>
+        <v>22.01</v>
       </c>
       <c r="E16" t="n">
         <v>129.14</v>
@@ -904,6 +915,7 @@
         <v>11815150592</v>
       </c>
       <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -912,13 +924,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>20.72</v>
+        <v>20.86</v>
       </c>
       <c r="C17" t="n">
-        <v>7.65</v>
+        <v>7.61</v>
       </c>
       <c r="D17" t="n">
-        <v>15.5</v>
+        <v>15.57</v>
       </c>
       <c r="E17" t="n">
         <v>64.65000000000001</v>
@@ -932,6 +944,7 @@
         <v>8883239936</v>
       </c>
       <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -940,13 +953,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>15.02</v>
+        <v>14.67</v>
       </c>
       <c r="C18" t="n">
-        <v>10.92</v>
+        <v>10.66</v>
       </c>
       <c r="D18" t="n">
-        <v>16.75</v>
+        <v>16.78</v>
       </c>
       <c r="E18" t="n">
         <v>71.02</v>
@@ -960,6 +973,7 @@
         <v>21288992768</v>
       </c>
       <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -968,13 +982,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>15.07</v>
+        <v>16.88</v>
       </c>
       <c r="C19" t="n">
-        <v>9.779999999999999</v>
+        <v>9.92</v>
       </c>
       <c r="D19" t="n">
-        <v>20.1</v>
+        <v>20.13</v>
       </c>
       <c r="E19" t="n">
         <v>84.41</v>
@@ -988,6 +1002,7 @@
         <v>11547899904</v>
       </c>
       <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -996,13 +1011,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17.5</v>
+        <v>18.84</v>
       </c>
       <c r="C20" t="n">
-        <v>7.16</v>
+        <v>7.14</v>
       </c>
       <c r="D20" t="n">
-        <v>17.2</v>
+        <v>17.25</v>
       </c>
       <c r="E20" t="n">
         <v>39.53</v>
@@ -1016,6 +1031,7 @@
         <v>138253320192</v>
       </c>
       <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1024,10 +1040,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3.46</v>
+        <v>-0.83</v>
       </c>
       <c r="C21" t="n">
-        <v>9.16</v>
+        <v>9.67</v>
       </c>
       <c r="D21" t="n">
         <v>17.14</v>
@@ -1036,7 +1052,7 @@
         <v>234.11</v>
       </c>
       <c r="F21" t="n">
-        <v>280.99</v>
+        <v>278.61</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -1044,6 +1060,7 @@
         <v>17671325696</v>
       </c>
       <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1052,13 +1069,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-2.77</v>
+        <v>-0.26</v>
       </c>
       <c r="C22" t="n">
-        <v>5.32</v>
+        <v>5.35</v>
       </c>
       <c r="D22" t="n">
-        <v>17.94</v>
+        <v>17.86</v>
       </c>
       <c r="E22" t="n">
         <v>76.92</v>
@@ -1072,6 +1089,7 @@
         <v>65681006592</v>
       </c>
       <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1080,13 +1098,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>14.72</v>
+        <v>16.49</v>
       </c>
       <c r="C23" t="n">
-        <v>13.97</v>
+        <v>14.03</v>
       </c>
       <c r="D23" t="n">
-        <v>19.65</v>
+        <v>19.68</v>
       </c>
       <c r="E23" t="n">
         <v>236.42</v>
@@ -1100,6 +1118,7 @@
         <v>2016758988800</v>
       </c>
       <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1108,13 +1127,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>16.72</v>
+        <v>18.46</v>
       </c>
       <c r="C24" t="n">
-        <v>11.25</v>
+        <v>11.27</v>
       </c>
       <c r="D24" t="n">
-        <v>17.04</v>
+        <v>17.06</v>
       </c>
       <c r="E24" t="n">
         <v>100.89</v>
@@ -1128,6 +1147,7 @@
         <v>70910558208</v>
       </c>
       <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1136,13 +1156,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>18.61</v>
+        <v>20.07</v>
       </c>
       <c r="C25" t="n">
-        <v>7.01</v>
+        <v>6.9</v>
       </c>
       <c r="D25" t="n">
-        <v>15.37</v>
+        <v>15.35</v>
       </c>
       <c r="E25" t="n">
         <v>102.76</v>
@@ -1156,6 +1176,7 @@
         <v>12185711616</v>
       </c>
       <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1164,13 +1185,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>10.89</v>
+        <v>13.49</v>
       </c>
       <c r="C26" t="n">
-        <v>2.83</v>
+        <v>2.73</v>
       </c>
       <c r="D26" t="n">
-        <v>13.77</v>
+        <v>13.68</v>
       </c>
       <c r="E26" t="n">
         <v>37.52</v>
@@ -1184,6 +1205,7 @@
         <v>3910768896</v>
       </c>
       <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1192,13 +1214,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-33.61</v>
+        <v>-39.71</v>
       </c>
       <c r="C27" t="n">
-        <v>-15.15</v>
+        <v>-15.38</v>
       </c>
       <c r="D27" t="n">
-        <v>91.53</v>
+        <v>91.45</v>
       </c>
       <c r="E27" t="n">
         <v>2.02</v>
@@ -1212,6 +1234,7 @@
         <v>880564416</v>
       </c>
       <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1220,13 +1243,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>9.24</v>
+        <v>10.43</v>
       </c>
       <c r="C28" t="n">
-        <v>8.65</v>
+        <v>9.07</v>
       </c>
       <c r="D28" t="n">
-        <v>31.63</v>
+        <v>31.65</v>
       </c>
       <c r="E28" t="n">
         <v>31.2</v>
@@ -1240,6 +1263,7 @@
         <v>178634816</v>
       </c>
       <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1248,13 +1272,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3.12</v>
+        <v>4.85</v>
       </c>
       <c r="C29" t="n">
-        <v>6.11</v>
+        <v>6.24</v>
       </c>
       <c r="D29" t="n">
-        <v>13.5</v>
+        <v>13.51</v>
       </c>
       <c r="E29" t="n">
         <v>49.94</v>
@@ -1268,6 +1292,7 @@
         <v>41319043072</v>
       </c>
       <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1276,13 +1301,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-1.96</v>
+        <v>1.91</v>
       </c>
       <c r="C30" t="n">
-        <v>10.51</v>
+        <v>10.74</v>
       </c>
       <c r="D30" t="n">
-        <v>18.41</v>
+        <v>18.43</v>
       </c>
       <c r="E30" t="n">
         <v>46.64</v>
@@ -1296,6 +1321,7 @@
         <v>19021103104</v>
       </c>
       <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1304,19 +1330,19 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>14.5</v>
+        <v>16.56</v>
       </c>
       <c r="C31" t="n">
-        <v>5.22</v>
+        <v>5.37</v>
       </c>
       <c r="D31" t="n">
-        <v>19.31</v>
+        <v>19.35</v>
       </c>
       <c r="E31" t="n">
         <v>52.48</v>
       </c>
       <c r="F31" t="n">
-        <v>73.39</v>
+        <v>73.5373</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
@@ -1324,6 +1350,7 @@
         <v>1376753152</v>
       </c>
       <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1332,13 +1359,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>27.44</v>
+        <v>29.66</v>
       </c>
       <c r="C32" t="n">
-        <v>9.44</v>
+        <v>9.6</v>
       </c>
       <c r="D32" t="n">
-        <v>19.08</v>
+        <v>19.1</v>
       </c>
       <c r="E32" t="n">
         <v>84.02</v>
@@ -1352,6 +1379,7 @@
         <v>27143948288</v>
       </c>
       <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1360,13 +1388,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.45</v>
+        <v>-0.72</v>
       </c>
       <c r="C33" t="n">
-        <v>7.64</v>
+        <v>7.37</v>
       </c>
       <c r="D33" t="n">
-        <v>13.65</v>
+        <v>13.63</v>
       </c>
       <c r="E33" t="n">
         <v>75.61</v>
@@ -1380,6 +1408,7 @@
         <v>16102211584</v>
       </c>
       <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1388,13 +1417,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-1.66</v>
+        <v>-0.78</v>
       </c>
       <c r="C34" t="n">
-        <v>6.64</v>
+        <v>6.65</v>
       </c>
       <c r="D34" t="n">
-        <v>24.66</v>
+        <v>24.68</v>
       </c>
       <c r="E34" t="n">
         <v>74.48999999999999</v>
@@ -1408,6 +1437,7 @@
         <v>26926057472</v>
       </c>
       <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1416,13 +1446,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>11.19</v>
+        <v>13.48</v>
       </c>
       <c r="C35" t="n">
-        <v>12.67</v>
+        <v>12.63</v>
       </c>
       <c r="D35" t="n">
-        <v>20.2</v>
+        <v>20.21</v>
       </c>
       <c r="E35" t="n">
         <v>42.21</v>
@@ -1436,6 +1466,7 @@
         <v>54020546560</v>
       </c>
       <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1444,19 +1475,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-4.77</v>
+        <v>-2.24</v>
       </c>
       <c r="C36" t="n">
-        <v>9.23</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>17.15</v>
+        <v>17.14</v>
       </c>
       <c r="E36" t="n">
         <v>127.35</v>
       </c>
       <c r="F36" t="n">
-        <v>153.14</v>
+        <v>151.39</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
@@ -1464,6 +1495,7 @@
         <v>34014875648</v>
       </c>
       <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1472,10 +1504,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10.62</v>
+        <v>14.7</v>
       </c>
       <c r="C37" t="n">
-        <v>13.19</v>
+        <v>13.03</v>
       </c>
       <c r="D37" t="n">
         <v>19.28</v>
@@ -1492,6 +1524,7 @@
         <v>23864965120</v>
       </c>
       <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1500,10 +1533,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.12</v>
+        <v>8.06</v>
       </c>
       <c r="C38" t="n">
-        <v>11.13</v>
+        <v>11.2</v>
       </c>
       <c r="D38" t="n">
         <v>17.37</v>
@@ -1520,6 +1553,7 @@
         <v>74538475520</v>
       </c>
       <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1528,19 +1562,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>23.45</v>
+        <v>24.8</v>
       </c>
       <c r="C39" t="n">
         <v>6.92</v>
       </c>
       <c r="D39" t="n">
-        <v>18.12</v>
+        <v>18.19</v>
       </c>
       <c r="E39" t="n">
         <v>30.565</v>
       </c>
       <c r="F39" t="n">
-        <v>44.4</v>
+        <v>44.61</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
@@ -1548,6 +1582,7 @@
         <v>5456395776</v>
       </c>
       <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1556,7 +1591,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4.64</v>
+        <v>7.07</v>
       </c>
       <c r="C40" t="n">
         <v>7.8</v>
@@ -1576,6 +1611,7 @@
         <v>1534526976</v>
       </c>
       <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1584,13 +1620,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>12.28</v>
+        <v>13.55</v>
       </c>
       <c r="C41" t="n">
-        <v>7.48</v>
+        <v>7.51</v>
       </c>
       <c r="D41" t="n">
-        <v>24.79</v>
+        <v>24.87</v>
       </c>
       <c r="E41" t="n">
         <v>22.26</v>
@@ -1604,6 +1640,7 @@
         <v>5694580224</v>
       </c>
       <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1612,13 +1649,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>29.05</v>
+        <v>29.6</v>
       </c>
       <c r="C42" t="n">
-        <v>4.62</v>
+        <v>4.53</v>
       </c>
       <c r="D42" t="n">
-        <v>28.4</v>
+        <v>28.41</v>
       </c>
       <c r="E42" t="n">
         <v>43.7</v>
@@ -1632,6 +1669,7 @@
         <v>8489536000</v>
       </c>
       <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1640,13 +1678,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>15.31</v>
+        <v>16.26</v>
       </c>
       <c r="C43" t="n">
-        <v>14.33</v>
+        <v>14.32</v>
       </c>
       <c r="D43" t="n">
-        <v>19.61</v>
+        <v>19.62</v>
       </c>
       <c r="E43" t="n">
         <v>89.16</v>
@@ -1660,6 +1698,7 @@
         <v>4951865344</v>
       </c>
       <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1668,10 +1707,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2.86</v>
+        <v>4.47</v>
       </c>
       <c r="C44" t="n">
-        <v>10.53</v>
+        <v>10.5</v>
       </c>
       <c r="D44" t="n">
         <v>13.17</v>
@@ -1688,6 +1727,7 @@
         <v>23435235328</v>
       </c>
       <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1696,13 +1736,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>7.1</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="C45" t="n">
-        <v>13.46</v>
+        <v>13.39</v>
       </c>
       <c r="D45" t="n">
-        <v>17.73</v>
+        <v>17.76</v>
       </c>
       <c r="E45" t="n">
         <v>148.34</v>
@@ -1716,6 +1756,7 @@
         <v>53128523776</v>
       </c>
       <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1724,13 +1765,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>17.69</v>
+        <v>20.09</v>
       </c>
       <c r="C46" t="n">
-        <v>7.67</v>
+        <v>7.69</v>
       </c>
       <c r="D46" t="n">
-        <v>16.69</v>
+        <v>16.66</v>
       </c>
       <c r="E46" t="n">
         <v>72.33</v>
@@ -1744,6 +1785,7 @@
         <v>10242850816</v>
       </c>
       <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1752,19 +1794,19 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4.21</v>
+        <v>7.3</v>
       </c>
       <c r="C47" t="n">
         <v>14.57</v>
       </c>
       <c r="D47" t="n">
-        <v>19.5</v>
+        <v>19.54</v>
       </c>
       <c r="E47" t="n">
         <v>75.43000000000001</v>
       </c>
       <c r="F47" t="n">
-        <v>101.82</v>
+        <v>102.76</v>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
@@ -1772,6 +1814,7 @@
         <v>12705400832</v>
       </c>
       <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1780,19 +1823,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>19.96</v>
+        <v>21.79</v>
       </c>
       <c r="C48" t="n">
-        <v>7.83</v>
+        <v>7.76</v>
       </c>
       <c r="D48" t="n">
-        <v>15.88</v>
+        <v>15.9</v>
       </c>
       <c r="E48" t="n">
         <v>53.65</v>
       </c>
       <c r="F48" t="n">
-        <v>72.95999999999999</v>
+        <v>73.02</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
@@ -1800,6 +1843,7 @@
         <v>74156916736</v>
       </c>
       <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1808,10 +1852,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>20.96</v>
+        <v>22.94</v>
       </c>
       <c r="C49" t="n">
-        <v>7.96</v>
+        <v>7.87</v>
       </c>
       <c r="D49" t="n">
         <v>16.27</v>
@@ -1828,6 +1872,7 @@
         <v>250765639680</v>
       </c>
       <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1836,13 +1881,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>20</v>
+        <v>21.56</v>
       </c>
       <c r="C50" t="n">
-        <v>7.93</v>
+        <v>7.88</v>
       </c>
       <c r="D50" t="n">
-        <v>17.1</v>
+        <v>17.07</v>
       </c>
       <c r="E50" t="n">
         <v>62.02</v>
@@ -1856,6 +1901,7 @@
         <v>35091558400</v>
       </c>
       <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1864,13 +1910,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>15.1</v>
+        <v>16.55</v>
       </c>
       <c r="C51" t="n">
-        <v>14.56</v>
+        <v>14.57</v>
       </c>
       <c r="D51" t="n">
-        <v>18.73</v>
+        <v>18.75</v>
       </c>
       <c r="E51" t="n">
         <v>442.8</v>
@@ -1884,6 +1930,7 @@
         <v>1409023475712</v>
       </c>
       <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1892,13 +1939,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>19.97</v>
+        <v>21.68</v>
       </c>
       <c r="C52" t="n">
-        <v>7.75</v>
+        <v>7.65</v>
       </c>
       <c r="D52" t="n">
-        <v>15.86</v>
+        <v>15.88</v>
       </c>
       <c r="E52" t="n">
         <v>54.98</v>
@@ -1912,6 +1959,7 @@
         <v>545534017536</v>
       </c>
       <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1920,19 +1968,19 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-8.19</v>
+        <v>-5.87</v>
       </c>
       <c r="C53" t="n">
-        <v>9.41</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="D53" t="n">
-        <v>19.95</v>
+        <v>19.96</v>
       </c>
       <c r="E53" t="n">
         <v>73.12</v>
       </c>
       <c r="F53" t="n">
-        <v>97.67</v>
+        <v>96.95999999999999</v>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
@@ -1940,6 +1988,7 @@
         <v>5462010368</v>
       </c>
       <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1948,13 +1997,13 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>18.5</v>
+        <v>22.35</v>
       </c>
       <c r="C54" t="n">
-        <v>12.77</v>
+        <v>12.91</v>
       </c>
       <c r="D54" t="n">
-        <v>24.86</v>
+        <v>24.88</v>
       </c>
       <c r="E54" t="n">
         <v>173.1</v>
@@ -1968,6 +2017,7 @@
         <v>24614813696</v>
       </c>
       <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1976,13 +2026,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>22.8</v>
+        <v>23.94</v>
       </c>
       <c r="C55" t="n">
-        <v>19.59</v>
+        <v>19.63</v>
       </c>
       <c r="D55" t="n">
-        <v>23.74</v>
+        <v>23.77</v>
       </c>
       <c r="E55" t="n">
         <v>402.39</v>
@@ -1996,6 +2046,7 @@
         <v>385755185152</v>
       </c>
       <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2004,10 +2055,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>22.04</v>
+        <v>23.16</v>
       </c>
       <c r="C56" t="n">
-        <v>14.77</v>
+        <v>14.92</v>
       </c>
       <c r="D56" t="n">
         <v>22.86</v>
@@ -2024,6 +2075,7 @@
         <v>19381745664</v>
       </c>
       <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2032,13 +2084,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>22.51</v>
+        <v>23.38</v>
       </c>
       <c r="C57" t="n">
-        <v>17.92</v>
+        <v>17.98</v>
       </c>
       <c r="D57" t="n">
-        <v>23.73</v>
+        <v>23.76</v>
       </c>
       <c r="E57" t="n">
         <v>308.67</v>
@@ -2052,6 +2104,7 @@
         <v>122123026432</v>
       </c>
       <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2060,13 +2113,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>24.21</v>
+        <v>25.21</v>
       </c>
       <c r="C58" t="n">
         <v>22.48</v>
       </c>
       <c r="D58" t="n">
-        <v>27.4</v>
+        <v>27.42</v>
       </c>
       <c r="E58" t="n">
         <v>172.45</v>
@@ -2080,6 +2133,7 @@
         <v>90249887744</v>
       </c>
       <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2088,19 +2142,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>36.91</v>
+        <v>37.8</v>
       </c>
       <c r="C59" t="n">
-        <v>30.41</v>
+        <v>30.12</v>
       </c>
       <c r="D59" t="n">
-        <v>37.53</v>
+        <v>37.55</v>
       </c>
       <c r="E59" t="n">
         <v>170.11</v>
       </c>
       <c r="F59" t="n">
-        <v>348.53</v>
+        <v>350.05</v>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
@@ -2108,6 +2162,7 @@
         <v>31551211520</v>
       </c>
       <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2116,13 +2171,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>22.53</v>
+        <v>23.63</v>
       </c>
       <c r="C60" t="n">
-        <v>17.24</v>
+        <v>17.32</v>
       </c>
       <c r="D60" t="n">
-        <v>23.81</v>
+        <v>23.85</v>
       </c>
       <c r="E60" t="n">
         <v>316.14</v>
@@ -2136,6 +2191,7 @@
         <v>342468952064</v>
       </c>
       <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2144,13 +2200,13 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>25.21</v>
+        <v>26.13</v>
       </c>
       <c r="C61" t="n">
-        <v>22.73</v>
+        <v>22.76</v>
       </c>
       <c r="D61" t="n">
-        <v>28.06</v>
+        <v>28.08</v>
       </c>
       <c r="E61" t="n">
         <v>451</v>
@@ -2164,6 +2220,7 @@
         <v>128300171264</v>
       </c>
       <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2172,10 +2229,10 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>6.68</v>
+        <v>9.17</v>
       </c>
       <c r="C62" t="n">
-        <v>9.83</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="D62" t="n">
         <v>16.15</v>
@@ -2192,6 +2249,7 @@
         <v>64171122688</v>
       </c>
       <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2200,13 +2258,13 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-3.11</v>
+        <v>-0.64</v>
       </c>
       <c r="C63" t="n">
-        <v>9.970000000000001</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="D63" t="n">
-        <v>15.62</v>
+        <v>15.59</v>
       </c>
       <c r="E63" t="n">
         <v>89.76000000000001</v>
@@ -2220,6 +2278,7 @@
         <v>11433600000</v>
       </c>
       <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2228,13 +2287,13 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-3.45</v>
+        <v>-0.79</v>
       </c>
       <c r="C64" t="n">
-        <v>11.36</v>
+        <v>11.25</v>
       </c>
       <c r="D64" t="n">
-        <v>16.21</v>
+        <v>16.18</v>
       </c>
       <c r="E64" t="n">
         <v>23.87</v>
@@ -2248,6 +2307,7 @@
         <v>71546724352</v>
       </c>
       <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2256,13 +2316,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>8.949999999999999</v>
+        <v>10.69</v>
       </c>
       <c r="C65" t="n">
-        <v>12.97</v>
+        <v>12.85</v>
       </c>
       <c r="D65" t="n">
-        <v>15.76</v>
+        <v>15.75</v>
       </c>
       <c r="E65" t="n">
         <v>169.32</v>
@@ -2276,6 +2336,7 @@
         <v>115132792832</v>
       </c>
       <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2284,13 +2345,13 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>9.5</v>
+        <v>11.25</v>
       </c>
       <c r="C66" t="n">
-        <v>11.13</v>
+        <v>11.03</v>
       </c>
       <c r="D66" t="n">
-        <v>15.76</v>
+        <v>15.75</v>
       </c>
       <c r="E66" t="n">
         <v>112.05</v>
@@ -2304,6 +2365,7 @@
         <v>81287471104</v>
       </c>
       <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2312,13 +2374,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>6.73</v>
+        <v>8.84</v>
       </c>
       <c r="C67" t="n">
-        <v>11.43</v>
+        <v>11.4</v>
       </c>
       <c r="D67" t="n">
-        <v>15.45</v>
+        <v>15.44</v>
       </c>
       <c r="E67" t="n">
         <v>150.43</v>
@@ -2332,6 +2394,7 @@
         <v>207800172544</v>
       </c>
       <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2340,10 +2403,10 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2.22</v>
+        <v>5.8</v>
       </c>
       <c r="C68" t="n">
-        <v>10.08</v>
+        <v>10.29</v>
       </c>
       <c r="D68" t="n">
         <v>21.4</v>
@@ -2360,6 +2423,7 @@
         <v>99760013312</v>
       </c>
       <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2368,13 +2432,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>8.69</v>
+        <v>11.79</v>
       </c>
       <c r="C69" t="n">
-        <v>10.68</v>
+        <v>10.81</v>
       </c>
       <c r="D69" t="n">
-        <v>17.94</v>
+        <v>17.95</v>
       </c>
       <c r="E69" t="n">
         <v>223.65</v>
@@ -2388,6 +2452,7 @@
         <v>201284747264</v>
       </c>
       <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2396,13 +2461,13 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1.51</v>
+        <v>5.88</v>
       </c>
       <c r="C70" t="n">
-        <v>9.25</v>
+        <v>9.5</v>
       </c>
       <c r="D70" t="n">
-        <v>23.5</v>
+        <v>23.48</v>
       </c>
       <c r="E70" t="n">
         <v>89.22</v>
@@ -2416,6 +2481,7 @@
         <v>85839454208</v>
       </c>
       <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2424,13 +2490,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>9.039999999999999</v>
+        <v>12.84</v>
       </c>
       <c r="C71" t="n">
-        <v>9.140000000000001</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="D71" t="n">
-        <v>23.51</v>
+        <v>23.53</v>
       </c>
       <c r="E71" t="n">
         <v>171.73</v>
@@ -2444,6 +2510,7 @@
         <v>70946291712</v>
       </c>
       <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2452,13 +2519,13 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.59</v>
+        <v>4.75</v>
       </c>
       <c r="C72" t="n">
-        <v>7.88</v>
+        <v>8.07</v>
       </c>
       <c r="D72" t="n">
-        <v>24.7</v>
+        <v>24.66</v>
       </c>
       <c r="E72" t="n">
         <v>74</v>
@@ -2472,6 +2539,7 @@
         <v>18618439680</v>
       </c>
       <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2480,19 +2548,19 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>5.47</v>
+        <v>6.47</v>
       </c>
       <c r="C73" t="n">
-        <v>1.89</v>
+        <v>1.91</v>
       </c>
       <c r="D73" t="n">
-        <v>4.97</v>
+        <v>4.92</v>
       </c>
       <c r="E73" t="n">
         <v>95.73999999999999</v>
       </c>
       <c r="F73" t="n">
-        <v>101.11</v>
+        <v>101.3499</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
@@ -2500,6 +2568,7 @@
         <v>131827171328</v>
       </c>
       <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2508,7 +2577,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>4.97</v>
+        <v>4.99</v>
       </c>
       <c r="C74" t="n">
         <v>2.47</v>
@@ -2528,6 +2597,7 @@
         <v>34145746944</v>
       </c>
       <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2536,19 +2606,19 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>5.3</v>
+        <v>5.61</v>
       </c>
       <c r="C75" t="n">
-        <v>1.97</v>
+        <v>1.98</v>
       </c>
       <c r="D75" t="n">
-        <v>2.13</v>
+        <v>2.11</v>
       </c>
       <c r="E75" t="n">
         <v>76.93000000000001</v>
       </c>
       <c r="F75" t="n">
-        <v>79.19</v>
+        <v>79.20999999999999</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
@@ -2556,6 +2626,7 @@
         <v>65453830144</v>
       </c>
       <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2564,19 +2635,19 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>5.38</v>
+        <v>6.33</v>
       </c>
       <c r="C76" t="n">
-        <v>1.96</v>
+        <v>1.97</v>
       </c>
       <c r="D76" t="n">
-        <v>4.9</v>
+        <v>4.85</v>
       </c>
       <c r="E76" t="n">
         <v>71.09999999999999</v>
       </c>
       <c r="F76" t="n">
-        <v>75</v>
+        <v>75.15000000000001</v>
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
@@ -2584,6 +2655,7 @@
         <v>374285697024</v>
       </c>
       <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2592,13 +2664,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>3.53</v>
+        <v>4.28</v>
       </c>
       <c r="C77" t="n">
-        <v>2.17</v>
+        <v>2.16</v>
       </c>
       <c r="D77" t="n">
-        <v>3.46</v>
+        <v>3.42</v>
       </c>
       <c r="E77" t="n">
         <v>48.29</v>
@@ -2612,6 +2684,7 @@
         <v>109574127616</v>
       </c>
       <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2620,13 +2693,11 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>6.11</v>
-      </c>
-      <c r="C78" t="n">
-        <v>4.43</v>
-      </c>
+        <v>5.69</v>
+      </c>
+      <c r="C78" t="inlineStr"/>
       <c r="D78" t="n">
-        <v>2.72</v>
+        <v>2.78</v>
       </c>
       <c r="E78" t="n">
         <v>44.3</v>
@@ -2640,6 +2711,7 @@
         <v>2409584128</v>
       </c>
       <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2648,13 +2720,11 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>6.62</v>
-      </c>
-      <c r="C79" t="n">
-        <v>4.3</v>
-      </c>
+        <v>6.68</v>
+      </c>
+      <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
-        <v>4.72</v>
+        <v>4.76</v>
       </c>
       <c r="E79" t="n">
         <v>39.49</v>
@@ -2668,6 +2738,7 @@
         <v>1702704256</v>
       </c>
       <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2676,19 +2747,19 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>6.11</v>
+        <v>6.47</v>
       </c>
       <c r="C80" t="n">
-        <v>2.7</v>
+        <v>2.71</v>
       </c>
       <c r="D80" t="n">
-        <v>2.36</v>
+        <v>2.35</v>
       </c>
       <c r="E80" t="n">
         <v>51.39</v>
       </c>
       <c r="F80" t="n">
-        <v>53.16</v>
+        <v>53.17</v>
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
@@ -2696,6 +2767,7 @@
         <v>21458319360</v>
       </c>
       <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2704,13 +2776,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>7.7</v>
+        <v>8.49</v>
       </c>
       <c r="C81" t="n">
-        <v>6.21</v>
+        <v>6.24</v>
       </c>
       <c r="D81" t="n">
-        <v>6.82</v>
+        <v>6.81</v>
       </c>
       <c r="E81" t="n">
         <v>24.82</v>
@@ -2724,6 +2796,7 @@
         <v>1849927936</v>
       </c>
       <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2732,13 +2805,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>7.17</v>
+        <v>7.81</v>
       </c>
       <c r="C82" t="n">
         <v>4.82</v>
       </c>
       <c r="D82" t="n">
-        <v>5.66</v>
+        <v>5.65</v>
       </c>
       <c r="E82" t="n">
         <v>75.08</v>
@@ -2752,6 +2825,7 @@
         <v>18542909440</v>
       </c>
       <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2760,19 +2834,19 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>5.91</v>
+        <v>7.35</v>
       </c>
       <c r="C83" t="n">
-        <v>3.07</v>
+        <v>3.04</v>
       </c>
       <c r="D83" t="n">
-        <v>7.24</v>
+        <v>7.17</v>
       </c>
       <c r="E83" t="n">
         <v>103.45</v>
       </c>
       <c r="F83" t="n">
-        <v>112.64</v>
+        <v>112.885</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
@@ -2780,6 +2854,7 @@
         <v>31793909760</v>
       </c>
       <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2788,13 +2863,13 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>7.02</v>
+        <v>7.78</v>
       </c>
       <c r="C84" t="n">
-        <v>4.78</v>
+        <v>4.81</v>
       </c>
       <c r="D84" t="n">
-        <v>5.84</v>
+        <v>5.83</v>
       </c>
       <c r="E84" t="n">
         <v>90.41</v>
@@ -2808,6 +2883,7 @@
         <v>8284786688</v>
       </c>
       <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2816,19 +2892,19 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>7.22</v>
+        <v>8.25</v>
       </c>
       <c r="C85" t="n">
-        <v>3.34</v>
+        <v>3.32</v>
       </c>
       <c r="D85" t="n">
-        <v>5.3</v>
+        <v>5.24</v>
       </c>
       <c r="E85" t="n">
         <v>78.66</v>
       </c>
       <c r="F85" t="n">
-        <v>84.73999999999999</v>
+        <v>84.8</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
@@ -2836,6 +2912,7 @@
         <v>58382168064</v>
       </c>
       <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2844,13 +2921,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>5.97</v>
+        <v>6.33</v>
       </c>
       <c r="C86" t="n">
-        <v>2.74</v>
+        <v>2.73</v>
       </c>
       <c r="D86" t="n">
-        <v>2.34</v>
+        <v>2.33</v>
       </c>
       <c r="E86" t="n">
         <v>77.58</v>
@@ -2864,6 +2941,7 @@
         <v>46178160640</v>
       </c>
       <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2872,13 +2950,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
       <c r="C87" t="n">
         <v>1.58</v>
       </c>
       <c r="D87" t="n">
-        <v>1.49</v>
+        <v>1.48</v>
       </c>
       <c r="E87" t="n">
         <v>81.67</v>
@@ -2892,6 +2970,7 @@
         <v>23979112448</v>
       </c>
       <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2900,13 +2979,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>1.45</v>
+        <v>4.05</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.38</v>
+        <v>-0.35</v>
       </c>
       <c r="D88" t="n">
-        <v>13.29</v>
+        <v>13.19</v>
       </c>
       <c r="E88" t="n">
         <v>83.3</v>
@@ -2920,6 +2999,7 @@
         <v>48818462720</v>
       </c>
       <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2928,19 +3008,19 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>5.45</v>
+        <v>6.7</v>
       </c>
       <c r="C89" t="n">
-        <v>1.12</v>
+        <v>1.15</v>
       </c>
       <c r="D89" t="n">
-        <v>6.07</v>
+        <v>6.02</v>
       </c>
       <c r="E89" t="n">
         <v>91.08</v>
       </c>
       <c r="F89" t="n">
-        <v>97.59</v>
+        <v>97.77</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
@@ -2948,6 +3028,7 @@
         <v>38510845952</v>
       </c>
       <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2956,19 +3037,19 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>9.630000000000001</v>
+        <v>11.6</v>
       </c>
       <c r="C90" t="n">
-        <v>3.49</v>
+        <v>3.6</v>
       </c>
       <c r="D90" t="n">
-        <v>7.16</v>
+        <v>7.1</v>
       </c>
       <c r="E90" t="n">
         <v>84.78</v>
       </c>
       <c r="F90" t="n">
-        <v>95.90000000000001</v>
+        <v>96.505</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
@@ -2976,6 +3057,7 @@
         <v>14815533056</v>
       </c>
       <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2984,7 +3066,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>4.33</v>
+        <v>4.34</v>
       </c>
       <c r="C91" t="n">
         <v>2.02</v>
@@ -3004,6 +3086,7 @@
         <v>20704555008</v>
       </c>
       <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3012,19 +3095,19 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>4.59</v>
+        <v>5.52</v>
       </c>
       <c r="C92" t="n">
-        <v>1.15</v>
+        <v>1.17</v>
       </c>
       <c r="D92" t="n">
-        <v>5.59</v>
+        <v>5.56</v>
       </c>
       <c r="E92" t="n">
         <v>22.23</v>
       </c>
       <c r="F92" t="n">
-        <v>23.34</v>
+        <v>23.36</v>
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr"/>
@@ -3032,6 +3115,7 @@
         <v>28781049856</v>
       </c>
       <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3040,7 +3124,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>4.29</v>
+        <v>4.28</v>
       </c>
       <c r="C93" t="n">
         <v>1.96</v>
@@ -3060,6 +3144,7 @@
         <v>42140692480</v>
       </c>
       <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3068,13 +3153,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>4.71</v>
+        <v>4.9</v>
       </c>
       <c r="C94" t="n">
         <v>1.66</v>
       </c>
       <c r="D94" t="n">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="E94" t="n">
         <v>58</v>
@@ -3088,6 +3173,7 @@
         <v>27585970176</v>
       </c>
       <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3099,7 +3185,7 @@
         <v>4.39</v>
       </c>
       <c r="C95" t="n">
-        <v>2.14</v>
+        <v>2.13</v>
       </c>
       <c r="D95" t="n">
         <v>0.29</v>
@@ -3116,6 +3202,7 @@
         <v>18063618048</v>
       </c>
       <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3124,10 +3211,10 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>11.07</v>
+        <v>11.45</v>
       </c>
       <c r="C96" t="n">
-        <v>2.22</v>
+        <v>2.25</v>
       </c>
       <c r="D96" t="n">
         <v>7.22</v>
@@ -3144,6 +3231,7 @@
         <v>3795501056</v>
       </c>
       <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3152,10 +3240,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>6.02</v>
+        <v>6.28</v>
       </c>
       <c r="C97" t="n">
-        <v>3.07</v>
+        <v>3.09</v>
       </c>
       <c r="D97" t="n">
         <v>1.98</v>
@@ -3172,6 +3260,7 @@
         <v>62167838720</v>
       </c>
       <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3180,13 +3269,13 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>5.15</v>
+        <v>6.09</v>
       </c>
       <c r="C98" t="n">
         <v>2.85</v>
       </c>
       <c r="D98" t="n">
-        <v>4.56</v>
+        <v>4.5</v>
       </c>
       <c r="E98" t="n">
         <v>106.04</v>
@@ -3200,6 +3289,7 @@
         <v>13950039040</v>
       </c>
       <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3208,19 +3298,19 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>6.19</v>
+        <v>7.23</v>
       </c>
       <c r="C99" t="n">
-        <v>1.38</v>
+        <v>1.4</v>
       </c>
       <c r="D99" t="n">
-        <v>5.56</v>
+        <v>5.51</v>
       </c>
       <c r="E99" t="n">
         <v>90.28</v>
       </c>
       <c r="F99" t="n">
-        <v>95.97</v>
+        <v>96.19799999999999</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
@@ -3228,6 +3318,7 @@
         <v>41748611072</v>
       </c>
       <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3236,13 +3327,13 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>2.73</v>
+        <v>3.51</v>
       </c>
       <c r="C100" t="n">
-        <v>2.23</v>
+        <v>2.24</v>
       </c>
       <c r="D100" t="n">
-        <v>4.72</v>
+        <v>4.7</v>
       </c>
       <c r="E100" t="n">
         <v>100.29</v>
@@ -3256,6 +3347,7 @@
         <v>39393619968</v>
       </c>
       <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3264,13 +3356,13 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2.81</v>
+        <v>3.54</v>
       </c>
       <c r="C101" t="n">
         <v>2.34</v>
       </c>
       <c r="D101" t="n">
-        <v>4.66</v>
+        <v>4.64</v>
       </c>
       <c r="E101" t="n">
         <v>47.02</v>
@@ -3284,6 +3376,7 @@
         <v>42452353024</v>
       </c>
       <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>